<commit_message>
24th Oct Sprint 2 Update
</commit_message>
<xml_diff>
--- a/docs/apis/api-descriptions.xlsx
+++ b/docs/apis/api-descriptions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\pet project\todo\apis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\Nodejs\todo\development-proccess\docs\apis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A39CAAC-E19C-409F-98AD-4B24BE0B64DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D78137-61F8-4D01-B003-73AB3848A0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{12C776B2-4C0A-487D-B4F3-922807601839}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{12C776B2-4C0A-487D-B4F3-922807601839}"/>
   </bookViews>
   <sheets>
     <sheet name="CONST" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="107">
   <si>
     <t>#</t>
   </si>
@@ -386,6 +386,15 @@
   </si>
   <si>
     <t>job_id</t>
+  </si>
+  <si>
+    <t>14-10-2024</t>
+  </si>
+  <si>
+    <t>Invalid status value</t>
+  </si>
+  <si>
+    <t>Internal Server error</t>
   </si>
 </sst>
 </file>
@@ -1319,7 +1328,7 @@
       </c>
       <c r="F5" s="19">
         <f ca="1">TODAY()</f>
-        <v>45573</v>
+        <v>45589</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
@@ -2196,8 +2205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CA9962-97FE-44DD-AEC4-91874CC7BF07}">
   <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2413,7 +2422,7 @@
     <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="9">
-        <f t="shared" ref="B10:B31" si="0">B9+1</f>
+        <f t="shared" ref="B10:B37" si="0">B9+1</f>
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -3088,14 +3097,25 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C31" s="9"/>
+      <c r="C31" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="F31" s="9">
         <f>COUNTIFS($C$8:C31, C31, $D$8:D31, D31, $E$8:E31, E31)</f>
-        <v>0</v>
-      </c>
-      <c r="G31" s="2" t="e">
+        <v>7</v>
+      </c>
+      <c r="G31" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(C31, CONST!$C$17:$D$19, 2, 0), "_",VLOOKUP(D31, CONST!$G$17:$H$18, 2, 0), VLOOKUP(E31, CONST!$K$17:$L$19, 2, 0), IF(F31 &lt; 10, "0"&amp;F31, F31) )</f>
-        <v>#N/A</v>
+        <v>ER_AU207</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
@@ -3105,9 +3125,30 @@
     </row>
     <row r="32" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="F32" s="9"/>
+      <c r="B32" s="9">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="9">
+        <f>COUNTIFS($C$8:C32, C32, $D$8:D32, D32, $E$8:E32, E32)</f>
+        <v>3</v>
+      </c>
+      <c r="G32" s="2" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(C32, CONST!$C$17:$D$19, 2, 0), "_",VLOOKUP(D32, CONST!$G$17:$H$18, 2, 0), VLOOKUP(E32, CONST!$K$17:$L$19, 2, 0), IF(F32 &lt; 10, "0"&amp;F32, F32) )</f>
+        <v>ER_UN103</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -3116,7 +3157,10 @@
     </row>
     <row r="33" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24"/>
-      <c r="B33" s="9"/>
+      <c r="B33" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
       <c r="C33" s="9"/>
       <c r="F33" s="9"/>
       <c r="I33" s="3"/>
@@ -3127,7 +3171,10 @@
     </row>
     <row r="34" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24"/>
-      <c r="B34" s="9"/>
+      <c r="B34" s="9">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
       <c r="C34" s="9"/>
       <c r="F34" s="9"/>
       <c r="I34" s="3"/>
@@ -3138,7 +3185,10 @@
     </row>
     <row r="35" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24"/>
-      <c r="B35" s="9"/>
+      <c r="B35" s="9">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
       <c r="C35" s="9"/>
       <c r="F35" s="9"/>
       <c r="I35" s="3"/>
@@ -3149,7 +3199,10 @@
     </row>
     <row r="36" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
-      <c r="B36" s="9"/>
+      <c r="B36" s="9">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
       <c r="C36" s="9"/>
       <c r="F36" s="9"/>
       <c r="I36" s="3"/>
@@ -3160,7 +3213,10 @@
     </row>
     <row r="37" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24"/>
-      <c r="B37" s="9"/>
+      <c r="B37" s="9">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
       <c r="C37" s="9"/>
       <c r="F37" s="9"/>
       <c r="I37" s="3"/>
@@ -3951,8 +4007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59BC092-5C84-474E-A7EA-21B518964950}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4026,9 +4082,8 @@
       <c r="E5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="19">
-        <f ca="1">TODAY()</f>
-        <v>45573</v>
+      <c r="F5" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
@@ -4200,7 +4255,7 @@
         <v>10</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4984,8 +5039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76081ECC-B795-4D24-987D-A8CD121982B5}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5060,7 +5115,7 @@
       </c>
       <c r="F5" s="19">
         <f ca="1">TODAY()</f>
-        <v>45573</v>
+        <v>45589</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="9"/>
@@ -5124,7 +5179,7 @@
         <v>36</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5150,7 +5205,7 @@
         <v>36</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5176,7 +5231,7 @@
         <v>36</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5202,7 +5257,7 @@
         <v>36</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5228,7 +5283,7 @@
         <v>36</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5309,11 +5364,28 @@
     </row>
     <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="F16" s="3"/>
+      <c r="B16" s="9">
+        <v>9</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>

</xml_diff>